<commit_message>
Updated first responder kit
</commit_message>
<xml_diff>
--- a/First-Responder-Kit/Worksheet - Sample SQL Server Inventory.xlsx
+++ b/First-Responder-Kit/Worksheet - Sample SQL Server Inventory.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brent/Dropbox (Brent Ozar Unlimited)/BOU Employees/Products/Download Pack/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="3920" yWindow="2500" windowWidth="43340" windowHeight="22760" tabRatio="500"/>
   </bookViews>
@@ -11,6 +16,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="77">
   <si>
     <t>http://www.BrentOzar.com</t>
   </si>
@@ -135,12 +143,6 @@
     <t>Current</t>
   </si>
   <si>
-    <t>RPO</t>
-  </si>
-  <si>
-    <t>RTO</t>
-  </si>
-  <si>
     <t>HA Current</t>
   </si>
   <si>
@@ -220,6 +222,42 @@
   </si>
   <si>
     <t>As of January 2015</t>
+  </si>
+  <si>
+    <t>RPO Goal</t>
+  </si>
+  <si>
+    <t>RTO Goal</t>
+  </si>
+  <si>
+    <t>Full Backups</t>
+  </si>
+  <si>
+    <t>Log Backups</t>
+  </si>
+  <si>
+    <t>Daily 11PM</t>
+  </si>
+  <si>
+    <t>Weekly Sat 9AM</t>
+  </si>
+  <si>
+    <t>Hourly</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>CHECKDB</t>
+  </si>
+  <si>
+    <t>Sat 10PM</t>
+  </si>
+  <si>
+    <t>Sat 11PM</t>
+  </si>
+  <si>
+    <t>Sun 2AM</t>
   </si>
 </sst>
 </file>
@@ -454,6 +492,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -779,16 +822,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AJ10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="8" width="10.83203125" hidden="1" customWidth="1"/>
@@ -796,32 +839,34 @@
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="9.83203125" hidden="1" customWidth="1"/>
     <col min="12" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="16" max="19" width="0" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="17.83203125" customWidth="1"/>
-    <col min="21" max="21" width="18.5" customWidth="1"/>
-    <col min="22" max="25" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="17.83203125" customWidth="1"/>
+    <col min="24" max="24" width="18.5" customWidth="1"/>
+    <col min="25" max="28" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="20" thickBot="1">
+    <row r="1" spans="1:36" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:33" ht="16" thickTop="1">
+    <row r="2" spans="1:36" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="C6" s="11" t="s">
         <v>3</v>
       </c>
@@ -838,37 +883,40 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
+        <v>56</v>
+      </c>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
-      <c r="T6" s="12" t="s">
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="13" t="s">
+      <c r="X6" s="5"/>
+      <c r="Y6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="14" t="s">
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
-      <c r="AF6" s="15" t="s">
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AG6" s="8"/>
+      <c r="AJ6" s="8"/>
     </row>
-    <row r="7" spans="1:33" ht="45">
+    <row r="7" spans="1:36" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
@@ -891,7 +939,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>10</v>
@@ -900,7 +948,7 @@
         <v>37</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L7" s="24" t="s">
         <v>35</v>
@@ -909,67 +957,76 @@
         <v>36</v>
       </c>
       <c r="N7" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="R7" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="S7" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="O7" s="25" t="s">
+      <c r="T7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="P7" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q7" s="25" t="s">
+      <c r="U7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="R7" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="S7" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="T7" s="20" t="s">
+      <c r="V7" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="W7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="U7" s="20" t="s">
+      <c r="X7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="V7" s="21" t="s">
+      <c r="Y7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="21" t="s">
+      <c r="Z7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="X7" s="21" t="s">
+      <c r="AA7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" s="21" t="s">
+      <c r="AB7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="Z7" s="22" t="s">
+      <c r="AC7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="AA7" s="22" t="s">
+      <c r="AD7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="AB7" s="22" t="s">
+      <c r="AE7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="AC7" s="22" t="s">
+      <c r="AF7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AD7" s="22" t="s">
+      <c r="AG7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="AE7" s="22" t="s">
+      <c r="AH7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AF7" s="23" t="s">
+      <c r="AI7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="AG7" s="23" t="s">
+      <c r="AJ7" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -977,7 +1034,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>90</v>
@@ -995,10 +1052,10 @@
         <v>17</v>
       </c>
       <c r="I8" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" t="s">
         <v>61</v>
-      </c>
-      <c r="J8" t="s">
-        <v>63</v>
       </c>
       <c r="K8" s="3">
         <v>41426</v>
@@ -1010,52 +1067,52 @@
         <v>17</v>
       </c>
       <c r="N8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>71</v>
+      </c>
+      <c r="R8" t="s">
+        <v>74</v>
+      </c>
+      <c r="S8" t="s">
+        <v>43</v>
+      </c>
+      <c r="T8" t="s">
+        <v>40</v>
+      </c>
+      <c r="U8" t="s">
         <v>55</v>
       </c>
-      <c r="O8" t="s">
-        <v>56</v>
-      </c>
-      <c r="P8" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>42</v>
-      </c>
-      <c r="R8" t="s">
-        <v>57</v>
-      </c>
-      <c r="S8" t="s">
-        <v>42</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" t="s">
         <v>18</v>
       </c>
-      <c r="U8" t="s">
-        <v>54</v>
-      </c>
-      <c r="V8" t="s">
-        <v>16</v>
-      </c>
-      <c r="W8" t="s">
-        <v>16</v>
-      </c>
       <c r="X8" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="Y8" t="s">
         <v>16</v>
       </c>
       <c r="Z8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AB8" t="s">
         <v>16</v>
       </c>
       <c r="AC8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD8" t="s">
         <v>16</v>
@@ -1064,21 +1121,30 @@
         <v>16</v>
       </c>
       <c r="AF8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AG8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>100</v>
@@ -1096,81 +1162,90 @@
         <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" t="s">
         <v>51</v>
       </c>
-      <c r="L9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" t="s">
-        <v>53</v>
-      </c>
       <c r="O9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P9" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="Q9" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="R9" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="S9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T9" t="s">
+        <v>40</v>
+      </c>
+      <c r="U9" t="s">
+        <v>55</v>
+      </c>
+      <c r="V9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" t="s">
+        <v>46</v>
+      </c>
+      <c r="X9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ9" t="s">
         <v>48</v>
       </c>
-      <c r="U9" t="s">
-        <v>49</v>
-      </c>
-      <c r="V9" t="s">
-        <v>16</v>
-      </c>
-      <c r="W9" t="s">
-        <v>16</v>
-      </c>
-      <c r="X9" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -1194,7 +1269,7 @@
         <v>17</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K10" s="3">
         <v>41275</v>
@@ -1206,49 +1281,49 @@
         <v>17</v>
       </c>
       <c r="N10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P10" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="Q10" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="R10" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="S10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="U10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="V10" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="W10" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="X10" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="Y10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AA10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AB10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AC10" t="s">
         <v>16</v>
@@ -1263,6 +1338,15 @@
         <v>16</v>
       </c>
       <c r="AG10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1272,10 +1356,5 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>